<commit_message>
Improving documentation on how to run Uppx.
</commit_message>
<xml_diff>
--- a/examples/simple-with-conf/simple-with-conf.xlsx
+++ b/examples/simple-with-conf/simple-with-conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/simple-with-conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4CEFBD-57D2-CC4D-A5C1-0371F50C8928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EBFA61-D0BE-0841-9541-726B68E988D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" activeTab="3" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
   <sheets>
     <sheet name="@Configurations" sheetId="15" r:id="rId1"/>
@@ -1073,14 +1073,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB81B79D-84CB-DC47-B910-0DBDA508B944}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="3" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="55" x14ac:dyDescent="0.25">
@@ -1093,6 +1094,7 @@
       <c r="C1" s="12" t="s">
         <v>196</v>
       </c>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1475,7 +1477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E766410-42AB-D842-913C-A2316B1EA100}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
experimenting with boolean expressions for features; small pretty print tweaks
</commit_message>
<xml_diff>
--- a/examples/simple-with-conf/simple-with-conf.xlsx
+++ b/examples/simple-with-conf/simple-with-conf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/simple-with-conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EBFA61-D0BE-0841-9541-726B68E988D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B98D2D6-E60A-D14A-A8ED-95D945550EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="196">
   <si>
     <t>Comment</t>
   </si>
@@ -614,9 +614,6 @@
   </si>
   <si>
     <t>Features</t>
-  </si>
-  <si>
-    <t>lazy</t>
   </si>
   <si>
     <t>Lazy worker</t>
@@ -1089,10 +1086,10 @@
         <v>186</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>195</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>196</v>
       </c>
       <c r="D1" s="12"/>
     </row>
@@ -1118,7 +1115,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>188</v>
@@ -1346,7 +1343,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1420,7 +1417,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1541,16 +1538,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
         <v>192</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>193</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>194</v>
-      </c>
-      <c r="D6" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2372,21 +2369,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA12DE6878FEE740AAE11B8EF5A3BEB8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ccf3f071624932fa9b6b142dc8790e1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf33d030-a745-437b-8efe-493a0e84c7f1" xmlns:ns3="38766943-c6ee-43fb-a1f1-f050a673c741" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fa4806b78295368f283e4cef5efe23" ns2:_="" ns3:_="">
     <xsd:import namespace="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
@@ -2597,10 +2579,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
+    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2623,20 +2631,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
-    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>